<commit_message>
Link dẫn đến tool check 3NF
</commit_message>
<xml_diff>
--- a/OrderInformation.xlsx
+++ b/OrderInformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tran Hai\HUST\20202\Database Lab\Project\Database-Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6810B3-CFB6-4981-8069-21631375B365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326EFFB9-4F54-45FE-99DD-B1A8C9F8DA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A022D5B-615A-41FF-ADB1-04E0E31071A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>OrderID</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>=&gt; TotalCost khong phu thuoc vao cac thuoc tinh cung hang</t>
+  </si>
+  <si>
+    <t>C,D không dẫn ra được F</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1920FA7A-D332-4633-89E8-590DD2F49EA1}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -499,6 +502,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>